<commit_message>
adding class 7 questions
</commit_message>
<xml_diff>
--- a/scripts/Prashant_Question.xlsx
+++ b/scripts/Prashant_Question.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SampleTest" sheetId="1" r:id="rId1"/>
-    <sheet name="StreamsChaptersTopics" sheetId="5" r:id="rId2"/>
-    <sheet name="Master" sheetId="2" r:id="rId3"/>
-    <sheet name="Latex Help" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
+    <sheet name="SampleTest6" sheetId="1" r:id="rId1"/>
+    <sheet name="SampleTest7" sheetId="6" r:id="rId2"/>
+    <sheet name="StreamsChaptersTopics" sheetId="5" r:id="rId3"/>
+    <sheet name="Master" sheetId="2" r:id="rId4"/>
+    <sheet name="Latex Help" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Latex Help'!$B$2:$B$301</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Master!$A$1:$K$302</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="3">'Latex Help'!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Latex Help'!$B$2:$B$301</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Master!$A$1:$K$302</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="4">'Latex Help'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3816" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4041" uniqueCount="970">
   <si>
     <t>Class</t>
   </si>
@@ -2574,6 +2575,381 @@
   </si>
   <si>
     <t>None of these</t>
+  </si>
+  <si>
+    <t>{tex} - {\text{45 }} \div {\text{ 9 }} = ?{/tex}</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>65958</t>
+  </si>
+  <si>
+    <t>65957</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>65956</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>65955</t>
+  </si>
+  <si>
+    <t>-5</t>
+  </si>
+  <si>
+    <t>{tex} - {\text{2 }} \times {\text{ }}\left( { - {\text{1}}} \right){\text{ }} = ?{/tex}</t>
+  </si>
+  <si>
+    <t>65975</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>65977</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>65978</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>65976</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>{tex}{\text{6 }} \times {\text{ }}\left( { - {\text{15}}} \right){\text{ }} = {\text{ }}\_\_\_\_\_\_{/tex}</t>
+  </si>
+  <si>
+    <t>65992</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>65994</t>
+  </si>
+  <si>
+    <t>-21</t>
+  </si>
+  <si>
+    <t>65991</t>
+  </si>
+  <si>
+    <t>-90</t>
+  </si>
+  <si>
+    <t>65993</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>{tex}\frac{1}{2}of10 = \_\_\_\_\_{/tex}</t>
+  </si>
+  <si>
+    <t>66401</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>66399</t>
+  </si>
+  <si>
+    <t>66402</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>66400</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>{tex}7 \div \frac{2}{5} = \_\_\_\_\_{/tex}</t>
+  </si>
+  <si>
+    <t>66409</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>66407</t>
+  </si>
+  <si>
+    <t>{tex}\frac{{35}}{2}{/tex}</t>
+  </si>
+  <si>
+    <t>66410</t>
+  </si>
+  <si>
+    <t>{tex}\frac{2}{{35}}{/tex}</t>
+  </si>
+  <si>
+    <t>66408</t>
+  </si>
+  <si>
+    <t>{tex}\frac{{37}}{5}{/tex}</t>
+  </si>
+  <si>
+    <t>A {tex}\_\_\_\_\_{/tex} is a fraction that represents a part of a whole.</t>
+  </si>
+  <si>
+    <t>66416</t>
+  </si>
+  <si>
+    <t>improper fraction</t>
+  </si>
+  <si>
+    <t>66415</t>
+  </si>
+  <si>
+    <t>proper fraction</t>
+  </si>
+  <si>
+    <t>66417</t>
+  </si>
+  <si>
+    <t>mixed fraction</t>
+  </si>
+  <si>
+    <t>66418</t>
+  </si>
+  <si>
+    <t>Find the ratio of Speed of a cycle 15 km per hour to the speed of scooter 30 km per hour.</t>
+  </si>
+  <si>
+    <t>69217</t>
+  </si>
+  <si>
+    <t>It is 1:3</t>
+  </si>
+  <si>
+    <t>69216</t>
+  </si>
+  <si>
+    <t>It is 2:1</t>
+  </si>
+  <si>
+    <t>69215</t>
+  </si>
+  <si>
+    <t>It is 1:2</t>
+  </si>
+  <si>
+    <t>69218</t>
+  </si>
+  <si>
+    <t>It is 3:1</t>
+  </si>
+  <si>
+    <t>Out of 32 students, 8 are absent. What percent of the students are present?</t>
+  </si>
+  <si>
+    <t>69236</t>
+  </si>
+  <si>
+    <t>69238</t>
+  </si>
+  <si>
+    <t>69237</t>
+  </si>
+  <si>
+    <t>69235</t>
+  </si>
+  <si>
+    <t>69261</t>
+  </si>
+  <si>
+    <t>Rs 40</t>
+  </si>
+  <si>
+    <t>69262</t>
+  </si>
+  <si>
+    <t>Rs 100</t>
+  </si>
+  <si>
+    <t>69259</t>
+  </si>
+  <si>
+    <t>Rs 80</t>
+  </si>
+  <si>
+    <t>69260</t>
+  </si>
+  <si>
+    <t>Rs 60</t>
+  </si>
+  <si>
+    <t>{tex}\_\_\_\_\_{/tex} is the multiplicative identity for rational numbers.</t>
+  </si>
+  <si>
+    <t>69671</t>
+  </si>
+  <si>
+    <t>69672</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>69674</t>
+  </si>
+  <si>
+    <t>69673</t>
+  </si>
+  <si>
+    <t>The sum of the rational numbers {tex}\frac{{ - 5}}{{16}}and\frac{7}{{12}}{/tex}is</t>
+  </si>
+  <si>
+    <t>69703</t>
+  </si>
+  <si>
+    <t>{tex}\frac{{13}}{{48}}{/tex}</t>
+  </si>
+  <si>
+    <t>69705</t>
+  </si>
+  <si>
+    <t>69704</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>69706</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>69797</t>
+  </si>
+  <si>
+    <t>{tex}\frac{8}{5}{/tex}</t>
+  </si>
+  <si>
+    <t>69796</t>
+  </si>
+  <si>
+    <t>{tex}\frac{5}{7}{/tex}</t>
+  </si>
+  <si>
+    <t>69798</t>
+  </si>
+  <si>
+    <t>69795</t>
+  </si>
+  <si>
+    <t>{tex}\frac{7}{5}{/tex}</t>
+  </si>
+  <si>
+    <t>Simplify and write in exponential form of {tex}{{\text{5}}^{\text{2}}} \times {\text{ }}{{\text{5}}^{\text{7}}} \times {\text{ }}{{\text{5}}^{{\text{12}}}}{/tex}</t>
+  </si>
+  <si>
+    <t>71400</t>
+  </si>
+  <si>
+    <t>{tex}{{\text{5}}^{{\text{12}}}}{/tex}</t>
+  </si>
+  <si>
+    <t>71401</t>
+  </si>
+  <si>
+    <t>{tex}{{\text{5}}^{{\text{18}}}}{/tex}</t>
+  </si>
+  <si>
+    <t>71402</t>
+  </si>
+  <si>
+    <t>71399</t>
+  </si>
+  <si>
+    <t>{tex}{{\text{5}}^{{\text{21}}}}{/tex}</t>
+  </si>
+  <si>
+    <t>Find the value of {tex}{\left( { - {\text{9}}} \right)^{\text{3}}} \times {\left( { - {\text{4}}} \right)^{\text{2}}}{/tex}.</t>
+  </si>
+  <si>
+    <t>71447</t>
+  </si>
+  <si>
+    <t>-11664</t>
+  </si>
+  <si>
+    <t>71448</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>71449</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>71450</t>
+  </si>
+  <si>
+    <t>Simplify and write the answer in exponential form. {tex}{{\text{5}}^{\text{8}}} \div {\text{ }}{{\text{5}}^{{\text{4}}}}{/tex}</t>
+  </si>
+  <si>
+    <t>71487</t>
+  </si>
+  <si>
+    <t>{tex}{{\text{5}}^{\text{4}}}{/tex}</t>
+  </si>
+  <si>
+    <t>71488</t>
+  </si>
+  <si>
+    <t>{tex}{{\text{5}}^{\text{3}}}{/tex}</t>
+  </si>
+  <si>
+    <t>71490</t>
+  </si>
+  <si>
+    <t>71489</t>
+  </si>
+  <si>
+    <t>{tex}{{\text{5}}^{\text{2}}}{/tex}</t>
+  </si>
+  <si>
+    <t>What number should be subtracted from{tex}\frac{{ - 3}}{5}to get - 2{/tex}?</t>
+  </si>
+  <si>
+    <t>Rahul bought a sweater and saved Rs 20 when a discount of {tex}25\% {/tex} was given. What was the price of the sweater before the discount?</t>
+  </si>
+  <si>
+    <t>{tex}50\% {/tex}</t>
+  </si>
+  <si>
+    <t>{tex}10\% {/tex}</t>
+  </si>
+  <si>
+    <t>{tex}25\% {/tex}</t>
+  </si>
+  <si>
+    <t>{tex}75\% {/tex}</t>
   </si>
 </sst>
 </file>
@@ -7201,8 +7577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7282,15 +7658,15 @@
         <v>21</v>
       </c>
       <c r="D2" t="str">
-        <f>IF(ISTEXT(C2),INDEX(Master!F2:F302,MATCH(SampleTest!C2,Master!H2:H302,0)),"")</f>
+        <f>IF(ISTEXT(C2),INDEX(Master!F2:F302,MATCH(SampleTest6!C2,Master!H2:H302,0)),"")</f>
         <v>Knowing the Numbers</v>
       </c>
       <c r="E2" t="str">
-        <f>IF(ISTEXT(C2),INDEX(Master!D2:D302,MATCH(SampleTest!C2,Master!H2:H302,0)),"")</f>
+        <f>IF(ISTEXT(C2),INDEX(Master!D2:D302,MATCH(SampleTest6!C2,Master!H2:H302,0)),"")</f>
         <v>Number System</v>
       </c>
       <c r="F2" t="str">
-        <f>IF(ISTEXT(C2),RIGHT(INDEX(Master!A2:A302,MATCH(SampleTest!C2,Master!H2:H302,0)),2),"")</f>
+        <f>IF(ISTEXT(C2),RIGHT(INDEX(Master!A2:A302,MATCH(SampleTest6!C2,Master!H2:H302,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G2">
@@ -7338,7 +7714,7 @@
         <v>14</v>
       </c>
       <c r="F3" t="str">
-        <f>IF(ISTEXT(C3),RIGHT(INDEX(Master!A3:A303,MATCH(SampleTest!C3,Master!H3:H303,0)),2),"")</f>
+        <f>IF(ISTEXT(C3),RIGHT(INDEX(Master!A3:A303,MATCH(SampleTest6!C3,Master!H3:H303,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G3">
@@ -7386,7 +7762,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="str">
-        <f>IF(ISTEXT(C4),RIGHT(INDEX(Master!A4:A304,MATCH(SampleTest!C4,Master!H4:H304,0)),2),"")</f>
+        <f>IF(ISTEXT(C4),RIGHT(INDEX(Master!A4:A304,MATCH(SampleTest6!C4,Master!H4:H304,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G4">
@@ -7434,7 +7810,7 @@
         <v>14</v>
       </c>
       <c r="F5" t="str">
-        <f>IF(ISTEXT(C5),RIGHT(INDEX(Master!A5:A305,MATCH(SampleTest!C5,Master!H5:H305,0)),2),"")</f>
+        <f>IF(ISTEXT(C5),RIGHT(INDEX(Master!A5:A305,MATCH(SampleTest6!C5,Master!H5:H305,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G5">
@@ -7482,7 +7858,7 @@
         <v>14</v>
       </c>
       <c r="F6" t="str">
-        <f>IF(ISTEXT(C6),RIGHT(INDEX(Master!A6:A306,MATCH(SampleTest!C6,Master!H6:H306,0)),2),"")</f>
+        <f>IF(ISTEXT(C6),RIGHT(INDEX(Master!A6:A306,MATCH(SampleTest6!C6,Master!H6:H306,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G6">
@@ -7530,7 +7906,7 @@
         <v>14</v>
       </c>
       <c r="F7" t="str">
-        <f>IF(ISTEXT(C7),RIGHT(INDEX(Master!A7:A307,MATCH(SampleTest!C7,Master!H7:H307,0)),2),"")</f>
+        <f>IF(ISTEXT(C7),RIGHT(INDEX(Master!A7:A307,MATCH(SampleTest6!C7,Master!H7:H307,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G7">
@@ -7578,7 +7954,7 @@
         <v>14</v>
       </c>
       <c r="F8" t="str">
-        <f>IF(ISTEXT(C8),RIGHT(INDEX(Master!A8:A308,MATCH(SampleTest!C8,Master!H8:H308,0)),2),"")</f>
+        <f>IF(ISTEXT(C8),RIGHT(INDEX(Master!A8:A308,MATCH(SampleTest6!C8,Master!H8:H308,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G8">
@@ -7626,7 +8002,7 @@
         <v>14</v>
       </c>
       <c r="F9" t="str">
-        <f>IF(ISTEXT(C9),RIGHT(INDEX(Master!A9:A309,MATCH(SampleTest!C9,Master!H9:H309,0)),2),"")</f>
+        <f>IF(ISTEXT(C9),RIGHT(INDEX(Master!A9:A309,MATCH(SampleTest6!C9,Master!H9:H309,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G9">
@@ -7674,7 +8050,7 @@
         <v>14</v>
       </c>
       <c r="F10" t="str">
-        <f>IF(ISTEXT(C10),RIGHT(INDEX(Master!A10:A310,MATCH(SampleTest!C10,Master!H10:H310,0)),2),"")</f>
+        <f>IF(ISTEXT(C10),RIGHT(INDEX(Master!A10:A310,MATCH(SampleTest6!C10,Master!H10:H310,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G10">
@@ -7722,7 +8098,7 @@
         <v>14</v>
       </c>
       <c r="F11" t="str">
-        <f>IF(ISTEXT(C11),RIGHT(INDEX(Master!A11:A311,MATCH(SampleTest!C11,Master!H11:H311,0)),2),"")</f>
+        <f>IF(ISTEXT(C11),RIGHT(INDEX(Master!A11:A311,MATCH(SampleTest6!C11,Master!H11:H311,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G11">
@@ -7770,7 +8146,7 @@
         <v>14</v>
       </c>
       <c r="F12" t="str">
-        <f>IF(ISTEXT(C12),RIGHT(INDEX(Master!A12:A312,MATCH(SampleTest!C12,Master!H12:H312,0)),2),"")</f>
+        <f>IF(ISTEXT(C12),RIGHT(INDEX(Master!A12:A312,MATCH(SampleTest6!C12,Master!H12:H312,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G12">
@@ -7818,7 +8194,7 @@
         <v>14</v>
       </c>
       <c r="F13" t="str">
-        <f>IF(ISTEXT(C13),RIGHT(INDEX(Master!A13:A313,MATCH(SampleTest!C13,Master!H13:H313,0)),2),"")</f>
+        <f>IF(ISTEXT(C13),RIGHT(INDEX(Master!A13:A313,MATCH(SampleTest6!C13,Master!H13:H313,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G13">
@@ -7866,7 +8242,7 @@
         <v>14</v>
       </c>
       <c r="F14" t="str">
-        <f>IF(ISTEXT(C14),RIGHT(INDEX(Master!A14:A314,MATCH(SampleTest!C14,Master!H14:H314,0)),2),"")</f>
+        <f>IF(ISTEXT(C14),RIGHT(INDEX(Master!A14:A314,MATCH(SampleTest6!C14,Master!H14:H314,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G14">
@@ -7914,7 +8290,7 @@
         <v>14</v>
       </c>
       <c r="F15" t="str">
-        <f>IF(ISTEXT(C15),RIGHT(INDEX(Master!A15:A315,MATCH(SampleTest!C15,Master!H15:H315,0)),2),"")</f>
+        <f>IF(ISTEXT(C15),RIGHT(INDEX(Master!A15:A315,MATCH(SampleTest6!C15,Master!H15:H315,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G15">
@@ -7962,7 +8338,7 @@
         <v>14</v>
       </c>
       <c r="F16" t="str">
-        <f>IF(ISTEXT(C16),RIGHT(INDEX(Master!A16:A316,MATCH(SampleTest!C16,Master!H16:H316,0)),2),"")</f>
+        <f>IF(ISTEXT(C16),RIGHT(INDEX(Master!A16:A316,MATCH(SampleTest6!C16,Master!H16:H316,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G16">
@@ -8010,7 +8386,7 @@
         <v>14</v>
       </c>
       <c r="F17" t="str">
-        <f>IF(ISTEXT(C17),RIGHT(INDEX(Master!A17:A317,MATCH(SampleTest!C17,Master!H17:H317,0)),2),"")</f>
+        <f>IF(ISTEXT(C17),RIGHT(INDEX(Master!A17:A317,MATCH(SampleTest6!C17,Master!H17:H317,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G17">
@@ -8058,7 +8434,7 @@
         <v>14</v>
       </c>
       <c r="F18" t="str">
-        <f>IF(ISTEXT(C18),RIGHT(INDEX(Master!A18:A318,MATCH(SampleTest!C18,Master!H18:H318,0)),2),"")</f>
+        <f>IF(ISTEXT(C18),RIGHT(INDEX(Master!A18:A318,MATCH(SampleTest6!C18,Master!H18:H318,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G18">
@@ -8106,7 +8482,7 @@
         <v>14</v>
       </c>
       <c r="F19" t="str">
-        <f>IF(ISTEXT(C19),RIGHT(INDEX(Master!A19:A319,MATCH(SampleTest!C19,Master!H19:H319,0)),2),"")</f>
+        <f>IF(ISTEXT(C19),RIGHT(INDEX(Master!A19:A319,MATCH(SampleTest6!C19,Master!H19:H319,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G19">
@@ -8154,7 +8530,7 @@
         <v>14</v>
       </c>
       <c r="F20" t="str">
-        <f>IF(ISTEXT(C20),RIGHT(INDEX(Master!A20:A320,MATCH(SampleTest!C20,Master!H20:H320,0)),2),"")</f>
+        <f>IF(ISTEXT(C20),RIGHT(INDEX(Master!A20:A320,MATCH(SampleTest6!C20,Master!H20:H320,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G20">
@@ -8202,7 +8578,7 @@
         <v>14</v>
       </c>
       <c r="F21" t="str">
-        <f>IF(ISTEXT(C21),RIGHT(INDEX(Master!A21:A321,MATCH(SampleTest!C21,Master!H21:H321,0)),2),"")</f>
+        <f>IF(ISTEXT(C21),RIGHT(INDEX(Master!A21:A321,MATCH(SampleTest6!C21,Master!H21:H321,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G21">
@@ -8250,7 +8626,7 @@
         <v>14</v>
       </c>
       <c r="F22" t="str">
-        <f>IF(ISTEXT(C22),RIGHT(INDEX(Master!A22:A322,MATCH(SampleTest!C22,Master!H22:H322,0)),2),"")</f>
+        <f>IF(ISTEXT(C22),RIGHT(INDEX(Master!A22:A322,MATCH(SampleTest6!C22,Master!H22:H322,0)),2),"")</f>
         <v>06</v>
       </c>
       <c r="G22">
@@ -8315,6 +8691,776 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="123.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B1" t="s">
+        <v>763</v>
+      </c>
+      <c r="C1" t="s">
+        <v>759</v>
+      </c>
+      <c r="D1" t="s">
+        <v>760</v>
+      </c>
+      <c r="E1" t="s">
+        <v>765</v>
+      </c>
+      <c r="F1" t="s">
+        <v>799</v>
+      </c>
+      <c r="G1" t="s">
+        <v>766</v>
+      </c>
+      <c r="H1" t="s">
+        <v>764</v>
+      </c>
+      <c r="I1" t="s">
+        <v>766</v>
+      </c>
+      <c r="J1" t="s">
+        <v>764</v>
+      </c>
+      <c r="K1" t="s">
+        <v>766</v>
+      </c>
+      <c r="L1" t="s">
+        <v>764</v>
+      </c>
+      <c r="M1" t="s">
+        <v>766</v>
+      </c>
+      <c r="N1" t="s">
+        <v>764</v>
+      </c>
+      <c r="O1" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>845</v>
+      </c>
+      <c r="C2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>846</v>
+      </c>
+      <c r="G2" t="s">
+        <v>847</v>
+      </c>
+      <c r="H2" t="s">
+        <v>844</v>
+      </c>
+      <c r="I2" t="s">
+        <v>848</v>
+      </c>
+      <c r="J2" t="s">
+        <v>849</v>
+      </c>
+      <c r="K2" t="s">
+        <v>850</v>
+      </c>
+      <c r="L2" t="s">
+        <v>851</v>
+      </c>
+      <c r="M2" t="s">
+        <v>852</v>
+      </c>
+      <c r="N2" t="s">
+        <v>853</v>
+      </c>
+      <c r="O2" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>854</v>
+      </c>
+      <c r="C3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>846</v>
+      </c>
+      <c r="G3" t="s">
+        <v>855</v>
+      </c>
+      <c r="H3" t="s">
+        <v>856</v>
+      </c>
+      <c r="I3" t="s">
+        <v>857</v>
+      </c>
+      <c r="J3" t="s">
+        <v>858</v>
+      </c>
+      <c r="K3" t="s">
+        <v>859</v>
+      </c>
+      <c r="L3" t="s">
+        <v>860</v>
+      </c>
+      <c r="M3" t="s">
+        <v>861</v>
+      </c>
+      <c r="N3" t="s">
+        <v>862</v>
+      </c>
+      <c r="O3" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>863</v>
+      </c>
+      <c r="C4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>846</v>
+      </c>
+      <c r="G4" t="s">
+        <v>864</v>
+      </c>
+      <c r="H4" t="s">
+        <v>865</v>
+      </c>
+      <c r="I4" t="s">
+        <v>866</v>
+      </c>
+      <c r="J4" t="s">
+        <v>867</v>
+      </c>
+      <c r="K4" t="s">
+        <v>868</v>
+      </c>
+      <c r="L4" t="s">
+        <v>869</v>
+      </c>
+      <c r="M4" t="s">
+        <v>870</v>
+      </c>
+      <c r="N4" t="s">
+        <v>871</v>
+      </c>
+      <c r="O4" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>872</v>
+      </c>
+      <c r="C5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>846</v>
+      </c>
+      <c r="G5" t="s">
+        <v>873</v>
+      </c>
+      <c r="H5" t="s">
+        <v>874</v>
+      </c>
+      <c r="I5" t="s">
+        <v>875</v>
+      </c>
+      <c r="J5" t="s">
+        <v>851</v>
+      </c>
+      <c r="K5" t="s">
+        <v>876</v>
+      </c>
+      <c r="L5" t="s">
+        <v>877</v>
+      </c>
+      <c r="M5" t="s">
+        <v>878</v>
+      </c>
+      <c r="N5" t="s">
+        <v>879</v>
+      </c>
+      <c r="O5" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>880</v>
+      </c>
+      <c r="C6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" t="s">
+        <v>246</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>846</v>
+      </c>
+      <c r="G6" t="s">
+        <v>881</v>
+      </c>
+      <c r="H6" t="s">
+        <v>882</v>
+      </c>
+      <c r="I6" t="s">
+        <v>883</v>
+      </c>
+      <c r="J6" t="s">
+        <v>884</v>
+      </c>
+      <c r="K6" t="s">
+        <v>885</v>
+      </c>
+      <c r="L6" t="s">
+        <v>886</v>
+      </c>
+      <c r="M6" t="s">
+        <v>887</v>
+      </c>
+      <c r="N6" t="s">
+        <v>888</v>
+      </c>
+      <c r="O6" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>889</v>
+      </c>
+      <c r="C7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>846</v>
+      </c>
+      <c r="G7" t="s">
+        <v>890</v>
+      </c>
+      <c r="H7" t="s">
+        <v>891</v>
+      </c>
+      <c r="I7" t="s">
+        <v>892</v>
+      </c>
+      <c r="J7" t="s">
+        <v>893</v>
+      </c>
+      <c r="K7" t="s">
+        <v>894</v>
+      </c>
+      <c r="L7" t="s">
+        <v>895</v>
+      </c>
+      <c r="M7" t="s">
+        <v>896</v>
+      </c>
+      <c r="N7" t="s">
+        <v>844</v>
+      </c>
+      <c r="O7" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>897</v>
+      </c>
+      <c r="C8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>846</v>
+      </c>
+      <c r="G8" t="s">
+        <v>898</v>
+      </c>
+      <c r="H8" t="s">
+        <v>899</v>
+      </c>
+      <c r="I8" t="s">
+        <v>900</v>
+      </c>
+      <c r="J8" t="s">
+        <v>901</v>
+      </c>
+      <c r="K8" t="s">
+        <v>902</v>
+      </c>
+      <c r="L8" t="s">
+        <v>903</v>
+      </c>
+      <c r="M8" t="s">
+        <v>904</v>
+      </c>
+      <c r="N8" t="s">
+        <v>905</v>
+      </c>
+      <c r="O8" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>906</v>
+      </c>
+      <c r="C9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" t="s">
+        <v>310</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>846</v>
+      </c>
+      <c r="G9" t="s">
+        <v>907</v>
+      </c>
+      <c r="H9" t="s">
+        <v>966</v>
+      </c>
+      <c r="I9" t="s">
+        <v>908</v>
+      </c>
+      <c r="J9" t="s">
+        <v>967</v>
+      </c>
+      <c r="K9" t="s">
+        <v>909</v>
+      </c>
+      <c r="L9" t="s">
+        <v>968</v>
+      </c>
+      <c r="M9" t="s">
+        <v>910</v>
+      </c>
+      <c r="N9" t="s">
+        <v>969</v>
+      </c>
+      <c r="O9" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>965</v>
+      </c>
+      <c r="C10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10" t="s">
+        <v>310</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>846</v>
+      </c>
+      <c r="G10" t="s">
+        <v>911</v>
+      </c>
+      <c r="H10" t="s">
+        <v>912</v>
+      </c>
+      <c r="I10" t="s">
+        <v>913</v>
+      </c>
+      <c r="J10" t="s">
+        <v>914</v>
+      </c>
+      <c r="K10" t="s">
+        <v>915</v>
+      </c>
+      <c r="L10" t="s">
+        <v>916</v>
+      </c>
+      <c r="M10" t="s">
+        <v>917</v>
+      </c>
+      <c r="N10" t="s">
+        <v>918</v>
+      </c>
+      <c r="O10" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>919</v>
+      </c>
+      <c r="C11" t="s">
+        <v>330</v>
+      </c>
+      <c r="D11" t="s">
+        <v>322</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>846</v>
+      </c>
+      <c r="G11" t="s">
+        <v>920</v>
+      </c>
+      <c r="H11" t="s">
+        <v>858</v>
+      </c>
+      <c r="I11" t="s">
+        <v>921</v>
+      </c>
+      <c r="J11" t="s">
+        <v>922</v>
+      </c>
+      <c r="K11" t="s">
+        <v>923</v>
+      </c>
+      <c r="L11" t="s">
+        <v>844</v>
+      </c>
+      <c r="M11" t="s">
+        <v>924</v>
+      </c>
+      <c r="N11" t="s">
+        <v>860</v>
+      </c>
+      <c r="O11" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>925</v>
+      </c>
+      <c r="C12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D12" t="s">
+        <v>322</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>846</v>
+      </c>
+      <c r="G12" t="s">
+        <v>926</v>
+      </c>
+      <c r="H12" t="s">
+        <v>927</v>
+      </c>
+      <c r="I12" t="s">
+        <v>928</v>
+      </c>
+      <c r="J12" t="s">
+        <v>877</v>
+      </c>
+      <c r="K12" t="s">
+        <v>929</v>
+      </c>
+      <c r="L12" t="s">
+        <v>930</v>
+      </c>
+      <c r="M12" t="s">
+        <v>931</v>
+      </c>
+      <c r="N12" t="s">
+        <v>932</v>
+      </c>
+      <c r="O12" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>964</v>
+      </c>
+      <c r="C13" t="s">
+        <v>330</v>
+      </c>
+      <c r="D13" t="s">
+        <v>322</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>846</v>
+      </c>
+      <c r="G13" t="s">
+        <v>933</v>
+      </c>
+      <c r="H13" t="s">
+        <v>934</v>
+      </c>
+      <c r="I13" t="s">
+        <v>935</v>
+      </c>
+      <c r="J13" t="s">
+        <v>936</v>
+      </c>
+      <c r="K13" t="s">
+        <v>937</v>
+      </c>
+      <c r="L13" t="s">
+        <v>844</v>
+      </c>
+      <c r="M13" t="s">
+        <v>938</v>
+      </c>
+      <c r="N13" t="s">
+        <v>939</v>
+      </c>
+      <c r="O13" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>940</v>
+      </c>
+      <c r="C14" t="s">
+        <v>368</v>
+      </c>
+      <c r="D14" t="s">
+        <v>364</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>846</v>
+      </c>
+      <c r="G14" t="s">
+        <v>941</v>
+      </c>
+      <c r="H14" t="s">
+        <v>942</v>
+      </c>
+      <c r="I14" t="s">
+        <v>943</v>
+      </c>
+      <c r="J14" t="s">
+        <v>944</v>
+      </c>
+      <c r="K14" t="s">
+        <v>945</v>
+      </c>
+      <c r="L14" t="s">
+        <v>844</v>
+      </c>
+      <c r="M14" t="s">
+        <v>946</v>
+      </c>
+      <c r="N14" t="s">
+        <v>947</v>
+      </c>
+      <c r="O14" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>948</v>
+      </c>
+      <c r="C15" t="s">
+        <v>368</v>
+      </c>
+      <c r="D15" t="s">
+        <v>364</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>846</v>
+      </c>
+      <c r="G15" t="s">
+        <v>949</v>
+      </c>
+      <c r="H15" t="s">
+        <v>950</v>
+      </c>
+      <c r="I15" t="s">
+        <v>951</v>
+      </c>
+      <c r="J15" t="s">
+        <v>952</v>
+      </c>
+      <c r="K15" t="s">
+        <v>953</v>
+      </c>
+      <c r="L15" t="s">
+        <v>954</v>
+      </c>
+      <c r="M15" t="s">
+        <v>955</v>
+      </c>
+      <c r="N15" t="s">
+        <v>844</v>
+      </c>
+      <c r="O15" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>956</v>
+      </c>
+      <c r="C16" t="s">
+        <v>368</v>
+      </c>
+      <c r="D16" t="s">
+        <v>364</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>846</v>
+      </c>
+      <c r="G16" t="s">
+        <v>957</v>
+      </c>
+      <c r="H16" t="s">
+        <v>958</v>
+      </c>
+      <c r="I16" t="s">
+        <v>959</v>
+      </c>
+      <c r="J16" t="s">
+        <v>960</v>
+      </c>
+      <c r="K16" t="s">
+        <v>961</v>
+      </c>
+      <c r="L16" t="s">
+        <v>844</v>
+      </c>
+      <c r="M16" t="s">
+        <v>962</v>
+      </c>
+      <c r="N16" t="s">
+        <v>963</v>
+      </c>
+      <c r="O16" t="s">
+        <v>957</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I261"/>
   <sheetViews>
     <sheetView topLeftCell="A224" workbookViewId="0">
@@ -11102,7 +12248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R302"/>
   <sheetViews>
@@ -30134,7 +31280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C301"/>
   <sheetViews>
@@ -31124,7 +32270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>